<commit_message>
Tiempos medición de inserción de datos con claves primarias y foráneas y sin las mismas
</commit_message>
<xml_diff>
--- a/ComparacionTiemposIndices.xlsx
+++ b/ComparacionTiemposIndices.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/Uni/3º/AdministraciónGestionBD/ABD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2844D373-E9F2-4549-8AB1-F85B5D7C30D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C19298-DD05-9945-8649-E946D438B286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{42C0C868-F13A-2045-927A-98E17B025AF7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{42C0C868-F13A-2045-927A-98E17B025AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>MEDIA</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>6B</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>Medición tiempos inserción post índices</t>
+  </si>
+  <si>
+    <t>Tiempos de medición insercción pre índices</t>
+  </si>
+  <si>
+    <t>SUMA</t>
   </si>
 </sst>
 </file>
@@ -560,15 +584,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5339B0E-0DD0-E440-A37C-5D6C657A6A9E}">
-  <dimension ref="B5:K45"/>
+  <dimension ref="B5:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -1561,6 +1587,233 @@
         <v>3.047619047619048E-2</v>
       </c>
     </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="2">
+        <v>4</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D49" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E49" s="7">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F49" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="3">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="D50" s="4">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B51" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="11">
+        <v>5.3E-3</v>
+      </c>
+      <c r="D51" s="11">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0</v>
+      </c>
+      <c r="F51" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="1">
+        <f>SUM(C49:C51)</f>
+        <v>2.35E-2</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" ref="D52:H52" si="37">SUM(D49:D51)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="37"/>
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="37"/>
+        <v>1.05</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="K52" s="1">
+        <f>AVERAGE(C52:I52)</f>
+        <v>0.28737499999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B54" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="2">
+        <v>4</v>
+      </c>
+      <c r="D54" s="2">
+        <v>5</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B55" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.64</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B56" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E56" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0.317</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B57" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="11">
+        <v>0</v>
+      </c>
+      <c r="D57" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="E57" s="11">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B58" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="1">
+        <f>SUM(C55:C57)</f>
+        <v>0.02</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" ref="D58:I58" si="38">SUM(D55:D57)</f>
+        <v>1.1199999999999999</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="38"/>
+        <v>0.44700000000000006</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="38"/>
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="I58" s="1">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="1">
+        <f>AVERAGE(C58:I58)</f>
+        <v>0.32142857142857145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>